<commit_message>
timer added in code. + results
</commit_message>
<xml_diff>
--- a/Results/Results/result analysis.xlsx
+++ b/Results/Results/result analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="baidu100" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="26">
   <si>
     <t>baidu100_w_sorted_f</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>50M</t>
+  </si>
+  <si>
+    <t>old result</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -1736,7 +1739,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,6 +1829,9 @@
         <f>F8/1000</f>
         <v>107.315</v>
       </c>
+      <c r="I8">
+        <v>426.31506899999999</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
@@ -1841,6 +1847,9 @@
         <f t="shared" ref="G9:G22" si="0">F9/1000</f>
         <v>114.27800000000001</v>
       </c>
+      <c r="I9">
+        <v>419.620991</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
@@ -1856,6 +1865,9 @@
         <f t="shared" si="0"/>
         <v>100.443</v>
       </c>
+      <c r="I10">
+        <v>431.43105500000001</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
@@ -1871,6 +1883,9 @@
         <f t="shared" si="0"/>
         <v>115.997</v>
       </c>
+      <c r="I11">
+        <v>418.57385599999998</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
@@ -1886,6 +1901,9 @@
         <f t="shared" si="0"/>
         <v>99.542000000000002</v>
       </c>
+      <c r="I12">
+        <v>427.36911800000001</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
@@ -1901,6 +1919,9 @@
         <f t="shared" si="0"/>
         <v>107.82899999999999</v>
       </c>
+      <c r="I13">
+        <v>429.038048</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
@@ -1916,6 +1937,9 @@
         <f t="shared" si="0"/>
         <v>135.22900000000001</v>
       </c>
+      <c r="I14">
+        <v>427.159786</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
@@ -1931,6 +1955,9 @@
         <f t="shared" si="0"/>
         <v>152.93700000000001</v>
       </c>
+      <c r="I15">
+        <v>426.05495500000001</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
@@ -1946,8 +1973,11 @@
         <f t="shared" si="0"/>
         <v>162.31800000000001</v>
       </c>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>424.33404899999999</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>19</v>
       </c>
@@ -1961,8 +1991,11 @@
         <f t="shared" si="0"/>
         <v>155.899</v>
       </c>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>420.593977</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>20</v>
       </c>
@@ -1976,8 +2009,11 @@
         <f t="shared" si="0"/>
         <v>160.541</v>
       </c>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>473.78492399999999</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>20</v>
       </c>
@@ -1991,8 +2027,11 @@
         <f t="shared" si="0"/>
         <v>277.38600000000002</v>
       </c>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>461.03119900000002</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>20</v>
       </c>
@@ -2006,8 +2045,11 @@
         <f t="shared" si="0"/>
         <v>371.00200000000001</v>
       </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>431.04291000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>20</v>
       </c>
@@ -2021,8 +2063,11 @@
         <f t="shared" si="0"/>
         <v>454.65199999999999</v>
       </c>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>408.66112700000002</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>20</v>
       </c>
@@ -2035,6 +2080,9 @@
       <c r="G22">
         <f t="shared" si="0"/>
         <v>501.73</v>
+      </c>
+      <c r="I22">
+        <v>406.934977</v>
       </c>
     </row>
   </sheetData>
@@ -2050,8 +2098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:G17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2363,10 +2411,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2382,7 +2430,7 @@
     <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2390,7 +2438,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2398,7 +2446,7 @@
         <v>2997166</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2406,7 +2454,7 @@
         <v>106349209</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="7" t="s">
@@ -2418,8 +2466,11 @@
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>4</v>
       </c>
@@ -2442,7 +2493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>18</v>
       </c>
@@ -2464,7 +2515,7 @@
         <v>668.00499000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>18</v>
       </c>
@@ -2486,7 +2537,7 @@
         <v>668.00499000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>18</v>
       </c>
@@ -2508,7 +2559,7 @@
         <v>668.00499000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>18</v>
       </c>
@@ -2530,7 +2581,7 @@
         <v>668.00499000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>18</v>
       </c>
@@ -2552,7 +2603,7 @@
         <v>668.00499000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>19</v>
       </c>
@@ -2569,15 +2620,15 @@
       <c r="I12">
         <v>668.00499000000002</v>
       </c>
-      <c r="J12">
-        <v>693.95279900000003</v>
-      </c>
       <c r="K12" s="5">
         <f t="shared" si="1"/>
-        <v>1361.957789</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L12">
+        <v>693.95279900000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>19</v>
       </c>
@@ -2594,15 +2645,15 @@
       <c r="I13">
         <v>668.00499000000002</v>
       </c>
-      <c r="J13">
-        <v>713.58394599999997</v>
-      </c>
       <c r="K13" s="5">
         <f t="shared" si="1"/>
-        <v>1381.5889360000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L13">
+        <v>713.58394599999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>19</v>
       </c>
@@ -2619,15 +2670,15 @@
       <c r="I14">
         <v>668.00499000000002</v>
       </c>
-      <c r="J14">
-        <v>669.58308199999999</v>
-      </c>
       <c r="K14" s="5">
         <f t="shared" si="1"/>
-        <v>1337.588072</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L14">
+        <v>669.58308199999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>19</v>
       </c>
@@ -2644,15 +2695,15 @@
       <c r="I15">
         <v>668.00499000000002</v>
       </c>
-      <c r="J15">
-        <v>678.76505899999995</v>
-      </c>
       <c r="K15" s="5">
         <f t="shared" si="1"/>
-        <v>1346.770049</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L15">
+        <v>678.76505899999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>19</v>
       </c>
@@ -2669,15 +2720,15 @@
       <c r="I16">
         <v>668.00499000000002</v>
       </c>
-      <c r="J16">
-        <v>661.39817200000005</v>
-      </c>
       <c r="K16" s="5">
         <f t="shared" si="1"/>
-        <v>1329.4031620000001</v>
-      </c>
-    </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L16">
+        <v>661.39817200000005</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>22</v>
       </c>
@@ -2694,15 +2745,15 @@
       <c r="I17">
         <v>668.00499000000002</v>
       </c>
-      <c r="J17">
-        <v>711.13109599999996</v>
-      </c>
       <c r="K17" s="5">
         <f t="shared" si="1"/>
-        <v>1379.136086</v>
-      </c>
-    </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L17">
+        <v>711.13109599999996</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>22</v>
       </c>
@@ -2719,15 +2770,15 @@
       <c r="I18">
         <v>668.00499000000002</v>
       </c>
-      <c r="J18">
-        <v>698.95195999999999</v>
-      </c>
       <c r="K18" s="5">
         <f t="shared" si="1"/>
-        <v>1366.95695</v>
-      </c>
-    </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L18">
+        <v>698.95195999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>22</v>
       </c>
@@ -2744,15 +2795,15 @@
       <c r="I19">
         <v>668.00499000000002</v>
       </c>
-      <c r="J19">
-        <v>706.68697399999996</v>
-      </c>
       <c r="K19" s="5">
         <f t="shared" si="1"/>
-        <v>1374.6919640000001</v>
-      </c>
-    </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L19">
+        <v>706.68697399999996</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>22</v>
       </c>
@@ -2769,15 +2820,15 @@
       <c r="I20">
         <v>668.00499000000002</v>
       </c>
-      <c r="J20">
-        <v>694.23413300000004</v>
-      </c>
       <c r="K20" s="5">
         <f t="shared" si="1"/>
-        <v>1362.2391230000001</v>
-      </c>
-    </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L20">
+        <v>694.23413300000004</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>22</v>
       </c>
@@ -2794,15 +2845,15 @@
       <c r="I21">
         <v>668.00499000000002</v>
       </c>
-      <c r="J21">
-        <v>684.23390400000005</v>
-      </c>
       <c r="K21" s="5">
         <f t="shared" si="1"/>
-        <v>1352.2388940000001</v>
-      </c>
-    </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L21">
+        <v>684.23390400000005</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>20</v>
       </c>
@@ -2819,15 +2870,15 @@
       <c r="I22">
         <v>668.00499000000002</v>
       </c>
-      <c r="J22">
-        <v>743.09015299999999</v>
-      </c>
       <c r="K22" s="5">
         <f t="shared" si="1"/>
-        <v>1411.095143</v>
-      </c>
-    </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L22">
+        <v>743.09015299999999</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>20</v>
       </c>
@@ -2844,15 +2895,15 @@
       <c r="I23">
         <v>668.00499000000002</v>
       </c>
-      <c r="J23">
-        <v>722.69701999999995</v>
-      </c>
       <c r="K23" s="5">
         <f t="shared" si="1"/>
-        <v>1390.70201</v>
-      </c>
-    </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L23">
+        <v>722.69701999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>20</v>
       </c>
@@ -2869,15 +2920,15 @@
       <c r="I24">
         <v>668.00499000000002</v>
       </c>
-      <c r="J24">
-        <v>695.26290900000004</v>
-      </c>
       <c r="K24" s="5">
         <f t="shared" si="1"/>
-        <v>1363.2678989999999</v>
-      </c>
-    </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L24">
+        <v>695.26290900000004</v>
+      </c>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>20</v>
       </c>
@@ -2894,15 +2945,15 @@
       <c r="I25">
         <v>668.00499000000002</v>
       </c>
-      <c r="J25">
-        <v>685.499191</v>
-      </c>
       <c r="K25" s="5">
         <f t="shared" si="1"/>
-        <v>1353.504181</v>
-      </c>
-    </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L25">
+        <v>685.499191</v>
+      </c>
+    </row>
+    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>20</v>
       </c>
@@ -2919,15 +2970,15 @@
       <c r="I26">
         <v>668.00499000000002</v>
       </c>
-      <c r="J26">
-        <v>669.27290000000005</v>
-      </c>
       <c r="K26" s="5">
         <f t="shared" si="1"/>
-        <v>1337.2778900000001</v>
-      </c>
-    </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L26">
+        <v>669.27290000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>24</v>
       </c>
@@ -2944,15 +2995,15 @@
       <c r="I27">
         <v>668.00499000000002</v>
       </c>
-      <c r="J27">
-        <v>944.73505</v>
-      </c>
       <c r="K27" s="5">
         <f t="shared" si="1"/>
-        <v>1612.7400400000001</v>
-      </c>
-    </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L27">
+        <v>944.73505</v>
+      </c>
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>24</v>
       </c>
@@ -2969,15 +3020,15 @@
       <c r="I28">
         <v>668.00499000000002</v>
       </c>
-      <c r="J28">
-        <v>851.50098800000001</v>
-      </c>
       <c r="K28" s="5">
         <f t="shared" si="1"/>
-        <v>1519.5059780000001</v>
-      </c>
-    </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L28">
+        <v>851.50098800000001</v>
+      </c>
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>24</v>
       </c>
@@ -2994,15 +3045,15 @@
       <c r="I29">
         <v>668.00499000000002</v>
       </c>
-      <c r="J29">
-        <v>806.025982</v>
-      </c>
       <c r="K29" s="5">
         <f t="shared" si="1"/>
-        <v>1474.030972</v>
-      </c>
-    </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L29">
+        <v>806.025982</v>
+      </c>
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>24</v>
       </c>
@@ -3019,15 +3070,15 @@
       <c r="I30">
         <v>668.00499000000002</v>
       </c>
-      <c r="J30">
-        <v>728.60503200000005</v>
-      </c>
       <c r="K30" s="5">
         <f t="shared" si="1"/>
-        <v>1396.6100220000001</v>
-      </c>
-    </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L30">
+        <v>728.60503200000005</v>
+      </c>
+    </row>
+    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>24</v>
       </c>
@@ -3044,12 +3095,12 @@
       <c r="I31">
         <v>668.00499000000002</v>
       </c>
-      <c r="J31">
-        <v>701.40504799999997</v>
-      </c>
       <c r="K31" s="5">
         <f t="shared" si="1"/>
-        <v>1369.410038</v>
+        <v>668.00499000000002</v>
+      </c>
+      <c r="L31">
+        <v>701.40504799999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>